<commit_message>
added comments to ~/idreamofsteel/util.py:getEstMaxTimeseries and created a demonstrative example in max.decay.xlsx
</commit_message>
<xml_diff>
--- a/helpers/max.decay.xlsx
+++ b/helpers/max.decay.xlsx
@@ -371,15 +371,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -387,7 +387,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -401,7 +401,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -418,7 +418,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>1</v>
       </c>
@@ -439,7 +439,7 @@
         <v>0.52473504881740241</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:10">
       <c r="A5">
         <f>A4+1</f>
         <v>2</v>
@@ -461,7 +461,7 @@
         <v>0.54934932549637516</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:10">
       <c r="A6">
         <f t="shared" ref="A6:A40" si="4">A5+1</f>
         <v>3</v>
@@ -483,7 +483,7 @@
         <v>0.57372440518115531</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:10">
       <c r="A7">
         <f t="shared" si="4"/>
         <v>4</v>
@@ -505,7 +505,7 @@
         <v>0.59774646129731634</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:10">
       <c r="A8">
         <f t="shared" si="4"/>
         <v>5</v>
@@ -527,7 +527,7 @@
         <v>0.62130833070177394</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:10">
       <c r="A9">
         <f t="shared" si="4"/>
         <v>6</v>
@@ -548,8 +548,15 @@
         <f t="shared" si="3"/>
         <v>0.64431131614916637</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="H9">
+        <f>455/0.89</f>
+        <v>511.23595505617976</v>
+      </c>
+      <c r="I9">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <f t="shared" si="4"/>
         <v>7</v>
@@ -570,8 +577,19 @@
         <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <f>C9</f>
+        <v>0.55204475683690624</v>
+      </c>
+      <c r="J10">
+        <f>I10+H10</f>
+        <v>1.5520447568369062</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <f t="shared" si="4"/>
         <v>8</v>
@@ -592,8 +610,20 @@
         <f t="shared" si="3"/>
         <v>0.6882966968253158</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="H11">
+        <f>H9*H10</f>
+        <v>511.23595505617976</v>
+      </c>
+      <c r="I11">
+        <f>I9*I10</f>
+        <v>245.65991679242327</v>
+      </c>
+      <c r="J11">
+        <f>SUM(H11:I11)/J10</f>
+        <v>487.67657537864426</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -615,7 +645,7 @@
         <v>0.70913552735484819</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:10">
       <c r="A13">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -636,8 +666,15 @@
         <f t="shared" si="3"/>
         <v>0.72912945022939057</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="H13">
+        <f>455/0.86</f>
+        <v>529.06976744186045</v>
+      </c>
+      <c r="I13">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -658,8 +695,19 @@
         <f t="shared" si="3"/>
         <v>0.74823693968561977</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <f>C9</f>
+        <v>0.55204475683690624</v>
+      </c>
+      <c r="J14">
+        <f>I14+H14</f>
+        <v>1.5520447568369062</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -680,8 +728,20 @@
         <f t="shared" si="3"/>
         <v>0.76642834547435423</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="H15">
+        <f>H13*H14</f>
+        <v>529.06976744186045</v>
+      </c>
+      <c r="I15">
+        <f>I13*I14</f>
+        <v>245.65991679242327</v>
+      </c>
+      <c r="J15">
+        <f>SUM(H15:I15)/J14</f>
+        <v>499.16710250881943</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
         <f t="shared" si="4"/>
         <v>13</v>

</xml_diff>